<commit_message>
Closing topic Nema opening Patients3MBq
</commit_message>
<xml_diff>
--- a/Matthias/01-NEMA_Phantom/Measured_vs_Simulated_allDosis_Mask_TK.xlsx
+++ b/Matthias/01-NEMA_Phantom/Measured_vs_Simulated_allDosis_Mask_TK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6984" tabRatio="703" activeTab="1" xr2:uid="{CEAB1AE0-CCC6-4F1C-87B6-462A97D959FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6990" tabRatio="703" xr2:uid="{CEAB1AE0-CCC6-4F1C-87B6-462A97D959FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim_vs_Mes-All_Dosis_MTK" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="D3_Compare" sheetId="11" r:id="rId7"/>
     <sheet name="D4_Compare" sheetId="12" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Which_Feature_to_be_watched!$A$1:$E$43</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -199,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="71">
   <si>
     <t>Jana Struct TextureFeature Zuordnung</t>
   </si>
@@ -381,10 +384,37 @@
     <t>ohne transformation</t>
   </si>
   <si>
-    <t>strong_relevant</t>
+    <t>GLCM - GTDSM 'Energy' or 'SecondAngularMoment'</t>
   </si>
   <si>
-    <t>relevant</t>
+    <t>GLCM or GTDSM 'Contrast'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GLCM or GTDSM 'Correlation'</t>
+  </si>
+  <si>
+    <t>GLCM or GTDSM  'SumAverage'</t>
+  </si>
+  <si>
+    <t>GLCM or GTDSM  'Entropy'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GLCM or GTDSM 'Variance'</t>
+  </si>
+  <si>
+    <t>GLCM or GTDSM  'Dissimilarity'</t>
+  </si>
+  <si>
+    <t>GLCM or GTDSM 'Homogeneity'</t>
+  </si>
+  <si>
+    <t>GLCM or GTDSM 'Energy'</t>
+  </si>
+  <si>
+    <t>relevant (r&gt;0,5)</t>
+  </si>
+  <si>
+    <t>strong_relevant p&lt;0,05</t>
   </si>
 </sst>
 </file>
@@ -538,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -717,12 +747,137 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -735,7 +890,7 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -829,45 +984,61 @@
     <xf numFmtId="11" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="15" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="15" xfId="2" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="2" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="6" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="2" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="6" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="15" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="9" borderId="15" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="20" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="15" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="20" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="6" fillId="5" borderId="15" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="20" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="6" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="6" fillId="5" borderId="20" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="6" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="6" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
@@ -2301,21 +2472,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C3EFAE-63B8-4ED6-8665-8A41871E76EB}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="13" customWidth="1"/>
-    <col min="3" max="10" width="12.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" style="34" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" style="27"/>
+    <col min="2" max="2" width="12.7109375" style="13" customWidth="1"/>
+    <col min="3" max="10" width="12.7109375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="13" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="34" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -2359,7 +2530,7 @@
       </c>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -2400,7 +2571,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -2437,7 +2608,7 @@
       <c r="N3" s="29"/>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -2474,9 +2645,9 @@
       <c r="N4" s="29"/>
       <c r="O4" s="22"/>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B5" s="9">
         <v>1.3416292925342601E-3</v>
@@ -2511,9 +2682,9 @@
       <c r="N5" s="30"/>
       <c r="O5" s="23"/>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B6" s="9">
         <v>82.941612976187997</v>
@@ -2548,9 +2719,9 @@
       <c r="N6" s="30"/>
       <c r="O6" s="23"/>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B7" s="9">
         <v>0.54137640003339005</v>
@@ -2585,9 +2756,9 @@
       <c r="N7" s="30"/>
       <c r="O7" s="23"/>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B8" s="9">
         <v>0.227737352063973</v>
@@ -2622,9 +2793,9 @@
       <c r="N8" s="30"/>
       <c r="O8" s="23"/>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B9" s="9">
         <v>4.8940948857609697E-3</v>
@@ -2659,9 +2830,9 @@
       <c r="N9" s="30"/>
       <c r="O9" s="23"/>
     </row>
-    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B10" s="9">
         <v>9.8703730932132991</v>
@@ -2696,9 +2867,9 @@
       <c r="N10" s="30"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B11" s="9">
         <v>2.2003700187942399E-2</v>
@@ -2733,9 +2904,9 @@
       <c r="N11" s="30"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B12" s="9">
         <v>7.0766290081309302</v>
@@ -2770,7 +2941,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="23"/>
     </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -2807,7 +2978,7 @@
       <c r="N13" s="31"/>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -2844,7 +3015,7 @@
       <c r="N14" s="31"/>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -2881,7 +3052,7 @@
       <c r="N15" s="31"/>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -2918,7 +3089,7 @@
       <c r="N16" s="31"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -2955,7 +3126,7 @@
       <c r="N17" s="31"/>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -2992,7 +3163,7 @@
       <c r="N18" s="31"/>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -3029,7 +3200,7 @@
       <c r="N19" s="31"/>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -3066,7 +3237,7 @@
       <c r="N20" s="31"/>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -3103,7 +3274,7 @@
       <c r="N21" s="31"/>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -3140,7 +3311,7 @@
       <c r="N22" s="31"/>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -3177,7 +3348,7 @@
       <c r="N23" s="32"/>
       <c r="O23" s="25"/>
     </row>
-    <row r="24" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -3214,7 +3385,7 @@
       <c r="N24" s="32"/>
       <c r="O24" s="25"/>
     </row>
-    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -3251,7 +3422,7 @@
       <c r="N25" s="32"/>
       <c r="O25" s="25"/>
     </row>
-    <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -3288,7 +3459,7 @@
       <c r="N26" s="31"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -3325,7 +3496,7 @@
       <c r="N27" s="31"/>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -3362,7 +3533,7 @@
       <c r="N28" s="31"/>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -3399,7 +3570,7 @@
       <c r="N29" s="32"/>
       <c r="O29" s="25"/>
     </row>
-    <row r="30" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -3436,7 +3607,7 @@
       <c r="N30" s="32"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -3473,7 +3644,7 @@
       <c r="N31" s="32"/>
       <c r="O31" s="25"/>
     </row>
-    <row r="32" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -3510,7 +3681,7 @@
       <c r="N32" s="32"/>
       <c r="O32" s="25"/>
     </row>
-    <row r="33" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -3547,7 +3718,7 @@
       <c r="N33" s="32"/>
       <c r="O33" s="25"/>
     </row>
-    <row r="34" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -3584,7 +3755,7 @@
       <c r="N34" s="32"/>
       <c r="O34" s="25"/>
     </row>
-    <row r="35" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -3621,7 +3792,7 @@
       <c r="N35" s="32"/>
       <c r="O35" s="25"/>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -3658,7 +3829,7 @@
       <c r="N36" s="32"/>
       <c r="O36" s="25"/>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -3695,7 +3866,7 @@
       <c r="N37" s="32"/>
       <c r="O37" s="25"/>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -3732,7 +3903,7 @@
       <c r="N38" s="32"/>
       <c r="O38" s="25"/>
     </row>
-    <row r="39" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -3769,7 +3940,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="26"/>
     </row>
-    <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -3806,7 +3977,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -3843,7 +4014,7 @@
       <c r="N41" s="33"/>
       <c r="O41" s="26"/>
     </row>
-    <row r="42" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -3880,7 +4051,7 @@
       <c r="N42" s="33"/>
       <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -3928,833 +4099,842 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEF64E8-C0CF-48B8-BA82-A098D67F4098}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="82" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="82"/>
-    <col min="4" max="4" width="19.6640625" style="83" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="83"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="69" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="69" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="70" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" style="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="83" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="B1" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="74"/>
+      <c r="D1" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="75"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="str">
+      <c r="B2" s="71" t="str">
         <f>IF(C2&lt;&gt;0,"Signifikant"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C2" s="82">
+      <c r="C2" s="71">
         <v>0</v>
       </c>
-      <c r="D2" s="83" t="str">
+      <c r="D2" s="72" t="str">
         <f>IF(E2&lt;&gt;0,"Interessant"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E2" s="83">
+      <c r="E2" s="78">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="str">
+      <c r="B3" s="69" t="str">
         <f t="shared" ref="B3:B42" si="0">IF(C3&lt;&gt;0,"Signifikant"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="69">
         <v>0</v>
       </c>
-      <c r="D3" s="83" t="str">
+      <c r="D3" s="70" t="str">
         <f t="shared" ref="D3:D43" si="1">IF(E3&lt;&gt;0,"Interessant"," ")</f>
         <v>Interessant</v>
       </c>
-      <c r="E3" s="83">
+      <c r="E3" s="80">
         <v>-0.84334340705856004</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="70" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82" t="str">
+      <c r="B4" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="69">
         <v>0</v>
       </c>
-      <c r="D4" s="83" t="str">
+      <c r="D4" s="70" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E4" s="83">
+      <c r="E4" s="80">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="82" t="str">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C5" s="82">
+      <c r="C5" s="69">
         <v>0.98094415724929396</v>
       </c>
-      <c r="D5" s="83" t="str">
+      <c r="D5" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E5" s="83">
+      <c r="E5" s="80">
         <v>0.98094415724929396</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="82" t="str">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C6" s="82">
+      <c r="C6" s="69">
         <v>0</v>
       </c>
-      <c r="D6" s="83" t="str">
+      <c r="D6" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E6" s="83">
+      <c r="E6" s="80">
         <v>0.90667141539436702</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="82" t="str">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="69">
         <v>0</v>
       </c>
-      <c r="D7" s="83" t="str">
+      <c r="D7" s="70" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E7" s="83">
+      <c r="E7" s="80">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="82" t="str">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="69">
         <v>0</v>
       </c>
-      <c r="D8" s="83" t="str">
+      <c r="D8" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="80">
         <v>0.78863358261163596</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="73" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="82" t="str">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C9" s="82">
+      <c r="C9" s="69">
         <v>0</v>
       </c>
-      <c r="D9" s="83" t="str">
+      <c r="D9" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="80">
         <v>0.94225755928788602</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="82" t="str">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="69">
         <v>0.983464848574366</v>
       </c>
-      <c r="D10" s="83" t="str">
+      <c r="D10" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="80">
         <v>0.983464848574366</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="82" t="str">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C11" s="82">
+      <c r="C11" s="69">
         <v>0.96852446011525595</v>
       </c>
-      <c r="D11" s="83" t="str">
+      <c r="D11" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="80">
         <v>0.96852446011525595</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="82" t="str">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C12" s="82">
+      <c r="C12" s="69">
         <v>0</v>
       </c>
-      <c r="D12" s="83" t="str">
+      <c r="D12" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="80">
         <v>0.880414083092942</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="74" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="82" t="str">
+      <c r="B13" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C13" s="82">
+      <c r="C13" s="69">
         <v>0</v>
       </c>
-      <c r="D13" s="83" t="str">
+      <c r="D13" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="80">
         <v>0.59865021210115799</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="82" t="str">
+      <c r="B14" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C14" s="82">
+      <c r="C14" s="69">
         <v>0</v>
       </c>
-      <c r="D14" s="83" t="str">
+      <c r="D14" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="80">
         <v>0.65352193986602303</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="74" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="82" t="str">
+      <c r="B15" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C15" s="82">
+      <c r="C15" s="69">
         <v>0.97674279578822198</v>
       </c>
-      <c r="D15" s="83" t="str">
+      <c r="D15" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E15" s="83">
+      <c r="E15" s="80">
         <v>0.97674279578822198</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="74" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="82" t="str">
+      <c r="B16" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C16" s="82">
+      <c r="C16" s="69">
         <v>0</v>
       </c>
-      <c r="D16" s="83" t="str">
+      <c r="D16" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E16" s="83">
+      <c r="E16" s="80">
         <v>0.58878704386803604</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="74" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="82" t="str">
+      <c r="B17" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C17" s="82">
+      <c r="C17" s="69">
         <v>0</v>
       </c>
-      <c r="D17" s="83" t="str">
+      <c r="D17" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E17" s="83">
+      <c r="E17" s="80">
         <v>0.62505964320140095</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="75" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="82" t="str">
+      <c r="B18" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C18" s="82">
+      <c r="C18" s="69">
         <v>-0.96788888686397101</v>
       </c>
-      <c r="D18" s="83" t="str">
+      <c r="D18" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E18" s="83">
+      <c r="E18" s="80">
         <v>-0.96788888686397101</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="74" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="82" t="str">
+      <c r="B19" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C19" s="82">
+      <c r="C19" s="69">
         <v>0.97351887955009098</v>
       </c>
-      <c r="D19" s="83" t="str">
+      <c r="D19" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E19" s="83">
+      <c r="E19" s="80">
         <v>0.97351887955009098</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="74" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="82" t="str">
+      <c r="B20" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C20" s="82">
+      <c r="C20" s="69">
         <v>0.96059237873661696</v>
       </c>
-      <c r="D20" s="83" t="str">
+      <c r="D20" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E20" s="83">
+      <c r="E20" s="80">
         <v>0.96059237873661696</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="74" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="82" t="str">
+      <c r="B21" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C21" s="82">
+      <c r="C21" s="69">
         <v>0</v>
       </c>
-      <c r="D21" s="83" t="str">
+      <c r="D21" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E21" s="83">
+      <c r="E21" s="80">
         <v>0.92409378832753297</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="74" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="82" t="str">
+      <c r="B22" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C22" s="82">
+      <c r="C22" s="69">
         <v>0.99973594679469802</v>
       </c>
-      <c r="D22" s="83" t="str">
+      <c r="D22" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E22" s="83">
+      <c r="E22" s="80">
         <v>0.99973594679469802</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="82" t="str">
+      <c r="B23" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C23" s="82">
+      <c r="C23" s="69">
         <v>0</v>
       </c>
-      <c r="D23" s="83" t="str">
+      <c r="D23" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E23" s="83">
+      <c r="E23" s="80">
         <v>0.71849382730993205</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="77" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="82" t="str">
+      <c r="B24" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C24" s="82">
+      <c r="C24" s="69">
         <v>0</v>
       </c>
-      <c r="D24" s="83" t="str">
+      <c r="D24" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E24" s="83">
+      <c r="E24" s="80">
         <v>0.64996905256680304</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="77" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="82" t="str">
+      <c r="B25" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C25" s="82">
+      <c r="C25" s="69">
         <v>0</v>
       </c>
-      <c r="D25" s="83" t="str">
+      <c r="D25" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E25" s="83">
+      <c r="E25" s="80">
         <v>0.93343263907822105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="82" t="str">
+      <c r="B26" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C26" s="82">
+      <c r="C26" s="69">
         <v>-0.98373744652900696</v>
       </c>
-      <c r="D26" s="83" t="str">
+      <c r="D26" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E26" s="83">
+      <c r="E26" s="80">
         <v>-0.98373744652900696</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="74" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="82" t="str">
+      <c r="B27" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C27" s="82">
+      <c r="C27" s="69">
         <v>0.97598760147302799</v>
       </c>
-      <c r="D27" s="83" t="str">
+      <c r="D27" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E27" s="83">
+      <c r="E27" s="80">
         <v>0.97598760147302799</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="74" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="82" t="str">
+      <c r="B28" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C28" s="82">
+      <c r="C28" s="69">
         <v>0</v>
       </c>
-      <c r="D28" s="83" t="str">
+      <c r="D28" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E28" s="83">
+      <c r="E28" s="80">
         <v>0.921403954645723</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="78" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="82" t="str">
+      <c r="B29" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C29" s="82">
+      <c r="C29" s="69">
         <v>0</v>
       </c>
-      <c r="D29" s="83" t="str">
+      <c r="D29" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E29" s="83">
+      <c r="E29" s="80">
         <v>0.70938857081172502</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="77" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="82" t="str">
+      <c r="B30" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C30" s="82">
+      <c r="C30" s="69">
         <v>0</v>
       </c>
-      <c r="D30" s="83" t="str">
+      <c r="D30" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E30" s="83">
+      <c r="E30" s="80">
         <v>0.53021105748659303</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="71" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="82" t="str">
+      <c r="B31" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C31" s="82">
+      <c r="C31" s="69">
         <v>0</v>
       </c>
-      <c r="D31" s="83" t="str">
+      <c r="D31" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E31" s="83">
+      <c r="E31" s="80">
         <v>0.50402048293739898</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="79" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="82" t="str">
+      <c r="B32" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C32" s="82">
+      <c r="C32" s="69">
         <v>0.98640124814101904</v>
       </c>
-      <c r="D32" s="83" t="str">
+      <c r="D32" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E32" s="83">
+      <c r="E32" s="80">
         <v>0.98640124814101904</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="71" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="82" t="str">
+      <c r="B33" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C33" s="82">
+      <c r="C33" s="69">
         <v>0</v>
       </c>
-      <c r="D33" s="83" t="str">
+      <c r="D33" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E33" s="83">
+      <c r="E33" s="80">
         <v>0.87951332144286598</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="80" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="82" t="str">
+      <c r="B34" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C34" s="82">
+      <c r="C34" s="69">
         <v>0.98441429728291097</v>
       </c>
-      <c r="D34" s="83" t="str">
+      <c r="D34" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E34" s="83">
+      <c r="E34" s="80">
         <v>0.98441429728291097</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="80" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="82" t="str">
+      <c r="B35" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C35" s="82">
+      <c r="C35" s="69">
         <v>0</v>
       </c>
-      <c r="D35" s="83" t="str">
+      <c r="D35" s="70" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E35" s="83">
+      <c r="E35" s="80">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="80" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="82" t="str">
+      <c r="B36" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C36" s="82">
+      <c r="C36" s="69">
         <v>0</v>
       </c>
-      <c r="D36" s="83" t="str">
+      <c r="D36" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E36" s="83">
+      <c r="E36" s="80">
         <v>-0.84437614994385801</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="80" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="82" t="str">
+      <c r="B37" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C37" s="82">
+      <c r="C37" s="69">
         <v>0</v>
       </c>
-      <c r="D37" s="83" t="str">
+      <c r="D37" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E37" s="83">
+      <c r="E37" s="80">
         <v>0.88985847317508604</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="80" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="82" t="str">
+      <c r="B38" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C38" s="82">
+      <c r="C38" s="69">
         <v>0</v>
       </c>
-      <c r="D38" s="83" t="str">
+      <c r="D38" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E38" s="83">
+      <c r="E38" s="80">
         <v>-0.55957873713127604</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="81" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="82" t="str">
+      <c r="B39" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C39" s="82">
+      <c r="C39" s="69">
         <v>0</v>
       </c>
-      <c r="D39" s="83" t="str">
+      <c r="D39" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E39" s="83">
+      <c r="E39" s="80">
         <v>0.59984490126308398</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="81" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="82" t="str">
+      <c r="B40" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C40" s="82">
+      <c r="C40" s="69">
         <v>0</v>
       </c>
-      <c r="D40" s="83" t="str">
+      <c r="D40" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E40" s="83">
+      <c r="E40" s="80">
         <v>0.94939894857966201</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="81" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="82" t="str">
+      <c r="B41" s="69" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C41" s="82">
+      <c r="C41" s="69">
         <v>0</v>
       </c>
-      <c r="D41" s="83" t="str">
+      <c r="D41" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E41" s="83">
+      <c r="E41" s="80">
         <v>0.887779232640306</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="81" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="82" t="str">
+      <c r="B42" s="69" t="str">
         <f t="shared" si="0"/>
         <v>Signifikant</v>
       </c>
-      <c r="C42" s="82">
+      <c r="C42" s="69">
         <v>0.97753699258675497</v>
       </c>
-      <c r="D42" s="83" t="str">
+      <c r="D42" s="70" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E42" s="83">
+      <c r="E42" s="80">
         <v>0.97753699258675497</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="81" t="s">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="82" t="str">
+      <c r="B43" s="93" t="str">
         <f>IF(C43&lt;&gt;0,"Signifikant"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C43" s="82">
+      <c r="C43" s="93">
         <v>0</v>
       </c>
-      <c r="D43" s="83" t="str">
+      <c r="D43" s="94" t="str">
         <f t="shared" si="1"/>
         <v>Interessant</v>
       </c>
-      <c r="E43" s="83">
+      <c r="E43" s="95">
         <v>0.79491795524470799</v>
       </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4766,15 +4946,15 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" style="60" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" style="62" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="58" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -4785,7 +4965,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -4800,7 +4980,7 @@
         <v>0.22100390029524827</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
@@ -4815,7 +4995,7 @@
         <v>-20.738395527237444</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -4830,7 +5010,7 @@
         <v>-2.8374759913231831</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>57</v>
       </c>
@@ -4845,7 +5025,7 @@
         <v>1.5289763834216858</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>5</v>
       </c>
@@ -4860,7 +5040,7 @@
         <v>2.9628655086972087</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>6</v>
       </c>
@@ -4875,7 +5055,7 @@
         <v>0.96632496296385195</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>7</v>
       </c>
@@ -4890,7 +5070,7 @@
         <v>0.98047604427471413</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -4905,7 +5085,7 @@
         <v>0.81663098920756272</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>9</v>
       </c>
@@ -4920,7 +5100,7 @@
         <v>0.8915843690456291</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -4935,7 +5115,7 @@
         <v>1.8538821007245201</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>11</v>
       </c>
@@ -4950,7 +5130,7 @@
         <v>2.5799069109485777</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -4965,7 +5145,7 @@
         <v>8.1141674582550873</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -4980,7 +5160,7 @@
         <v>0.6730437252298882</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -4995,7 +5175,7 @@
         <v>0.53079394521493595</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -5010,7 +5190,7 @@
         <v>4.731792326014487</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -5025,7 +5205,7 @@
         <v>1.7005796902810768</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -5040,7 +5220,7 @@
         <v>0.65559777286450649</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -5055,7 +5235,7 @@
         <v>2.6986414747414047</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -5070,7 +5250,7 @@
         <v>0.25976781062598786</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -5085,7 +5265,7 @@
         <v>13.372416259839857</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -5100,7 +5280,7 @@
         <v>0.61038626160105325</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="54" t="s">
         <v>22</v>
       </c>
@@ -5115,7 +5295,7 @@
         <v>10857807428.36091</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -5130,7 +5310,7 @@
         <v>1.1401258236302761E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -5145,7 +5325,7 @@
         <v>0.75224966808175997</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -5160,7 +5340,7 @@
         <v>2.7117620565402185</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -5175,7 +5355,7 @@
         <v>28.081324955208988</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -5190,7 +5370,7 @@
         <v>1.251657275145535</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
         <v>28</v>
       </c>
@@ -5205,7 +5385,7 @@
         <v>0.35466898326476398</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -5220,7 +5400,7 @@
         <v>124.71569979779608</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="53" t="s">
         <v>30</v>
       </c>
@@ -5235,7 +5415,7 @@
         <v>0.4856050382366176</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="57" t="s">
         <v>31</v>
       </c>
@@ -5250,7 +5430,7 @@
         <v>4.1538461538461595</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
         <v>32</v>
       </c>
@@ -5265,7 +5445,7 @@
         <v>3746612192.0750699</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -5280,7 +5460,7 @@
         <v>54431080203.797195</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -5295,7 +5475,7 @@
         <v>1.9515437015490144E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -5310,7 +5490,7 @@
         <v>4.5640310354127748E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -5325,7 +5505,7 @@
         <v>0.5669448606432177</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -5340,7 +5520,7 @@
         <v>5.865728178013417E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -5355,7 +5535,7 @@
         <v>1.7834100925449967</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -5370,7 +5550,7 @@
         <v>0.76630452864961585</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -5385,7 +5565,7 @@
         <v>0.14445492813477548</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -5400,7 +5580,7 @@
         <v>8.4496932746363491</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -5429,17 +5609,17 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="27"/>
+    <col min="2" max="2" width="12.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -5461,7 +5641,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -5478,7 +5658,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -5491,7 +5671,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -5504,7 +5684,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -5517,7 +5697,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -5530,7 +5710,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -5543,7 +5723,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -5556,7 +5736,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -5569,7 +5749,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -5582,7 +5762,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -5595,7 +5775,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -5608,7 +5788,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -5621,7 +5801,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -5634,7 +5814,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -5647,7 +5827,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -5660,7 +5840,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -5673,7 +5853,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -5686,7 +5866,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -5699,7 +5879,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -5712,7 +5892,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -5725,7 +5905,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -5738,7 +5918,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -5751,7 +5931,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -5764,7 +5944,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -5777,7 +5957,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -5790,7 +5970,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -5803,7 +5983,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -5816,7 +5996,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -5829,7 +6009,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -5842,7 +6022,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -5855,7 +6035,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -5868,7 +6048,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -5881,7 +6061,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -5894,7 +6074,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -5907,7 +6087,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -5920,7 +6100,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -5933,7 +6113,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -5946,7 +6126,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -5959,7 +6139,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -5972,7 +6152,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -5985,7 +6165,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -5998,7 +6178,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -6028,16 +6208,16 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="12.77734375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="27"/>
+    <col min="2" max="3" width="12.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -6059,7 +6239,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -6076,7 +6256,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -6089,7 +6269,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -6102,7 +6282,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -6115,7 +6295,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -6128,7 +6308,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -6141,7 +6321,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -6154,7 +6334,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -6167,7 +6347,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -6180,7 +6360,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -6193,7 +6373,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -6206,7 +6386,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -6219,7 +6399,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -6232,7 +6412,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -6245,7 +6425,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -6258,7 +6438,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -6271,7 +6451,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -6284,7 +6464,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -6297,7 +6477,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -6310,7 +6490,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -6323,7 +6503,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -6336,7 +6516,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -6349,7 +6529,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -6362,7 +6542,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -6375,7 +6555,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -6388,7 +6568,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -6401,7 +6581,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -6414,7 +6594,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -6427,7 +6607,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -6440,7 +6620,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -6453,7 +6633,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -6466,7 +6646,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -6479,7 +6659,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -6492,7 +6672,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -6505,7 +6685,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -6518,7 +6698,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -6531,7 +6711,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -6544,7 +6724,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -6557,7 +6737,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -6570,7 +6750,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -6583,7 +6763,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -6596,7 +6776,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -6626,16 +6806,16 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="12.77734375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="27"/>
+    <col min="2" max="3" width="12.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -6657,7 +6837,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -6674,7 +6854,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -6687,7 +6867,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -6700,7 +6880,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -6713,7 +6893,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -6726,7 +6906,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -6739,7 +6919,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -6752,7 +6932,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -6765,7 +6945,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -6778,7 +6958,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -6791,7 +6971,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -6804,7 +6984,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -6817,7 +6997,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -6830,7 +7010,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -6843,7 +7023,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -6856,7 +7036,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -6869,7 +7049,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -6882,7 +7062,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -6895,7 +7075,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -6908,7 +7088,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -6921,7 +7101,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -6934,7 +7114,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -6947,7 +7127,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -6960,7 +7140,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -6973,7 +7153,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -6986,7 +7166,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -6999,7 +7179,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -7012,7 +7192,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -7025,7 +7205,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -7038,7 +7218,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -7051,7 +7231,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -7064,7 +7244,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -7077,7 +7257,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -7090,7 +7270,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -7103,7 +7283,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -7116,7 +7296,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -7129,7 +7309,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -7142,7 +7322,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -7155,7 +7335,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -7168,7 +7348,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -7181,7 +7361,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -7194,7 +7374,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -7224,16 +7404,16 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="12.77734375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="27"/>
+    <col min="2" max="3" width="12.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -7255,7 +7435,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -7272,7 +7452,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -7285,7 +7465,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -7298,7 +7478,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -7311,7 +7491,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -7324,7 +7504,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -7337,7 +7517,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -7350,7 +7530,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -7363,7 +7543,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -7376,7 +7556,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -7389,7 +7569,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -7402,7 +7582,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -7415,7 +7595,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -7428,7 +7608,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -7441,7 +7621,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -7454,7 +7634,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -7467,7 +7647,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -7480,7 +7660,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -7493,7 +7673,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -7506,7 +7686,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -7519,7 +7699,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -7532,7 +7712,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -7545,7 +7725,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -7558,7 +7738,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -7571,7 +7751,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -7584,7 +7764,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -7597,7 +7777,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -7610,7 +7790,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -7623,7 +7803,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -7636,7 +7816,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -7649,7 +7829,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -7662,7 +7842,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -7675,7 +7855,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -7688,7 +7868,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -7701,7 +7881,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -7714,7 +7894,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -7727,7 +7907,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -7740,7 +7920,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -7753,7 +7933,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -7766,7 +7946,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -7779,7 +7959,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -7792,7 +7972,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -7822,17 +8002,17 @@
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="19" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="27"/>
+    <col min="2" max="2" width="12.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -7854,7 +8034,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -7871,7 +8051,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -7884,7 +8064,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -7897,7 +8077,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -7910,7 +8090,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -7923,7 +8103,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -7936,7 +8116,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -7949,7 +8129,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -7962,7 +8142,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -7975,7 +8155,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -7988,7 +8168,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -8001,7 +8181,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -8014,7 +8194,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -8027,7 +8207,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -8040,7 +8220,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -8053,7 +8233,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -8066,7 +8246,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -8079,7 +8259,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -8092,7 +8272,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -8105,7 +8285,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -8118,7 +8298,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -8131,7 +8311,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -8144,7 +8324,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -8157,7 +8337,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -8170,7 +8350,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -8183,7 +8363,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -8196,7 +8376,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -8209,7 +8389,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -8222,7 +8402,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -8235,7 +8415,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -8248,7 +8428,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -8261,7 +8441,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -8274,7 +8454,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -8287,7 +8467,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -8300,7 +8480,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -8313,7 +8493,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -8326,7 +8506,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -8339,7 +8519,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -8352,7 +8532,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -8365,7 +8545,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -8378,7 +8558,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -8391,7 +8571,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
.nii Einzelmasken können geladen werden
</commit_message>
<xml_diff>
--- a/Matthias/01-NEMA_Phantom/Measured_vs_Simulated_allDosis_Mask_TK.xlsx
+++ b/Matthias/01-NEMA_Phantom/Measured_vs_Simulated_allDosis_Mask_TK.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\TAToolbox\Matthias\01-NEMA_Phantom\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391EA5BA-6836-45FC-831D-D68F53510FA3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6990" tabRatio="703" xr2:uid="{CEAB1AE0-CCC6-4F1C-87B6-462A97D959FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6996" tabRatio="703" activeTab="2" xr2:uid="{CEAB1AE0-CCC6-4F1C-87B6-462A97D959FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim_vs_Mes-All_Dosis_MTK" sheetId="4" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="D4_Compare" sheetId="12" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Which_Feature_to_be_watched!$A$1:$E$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Which_Feature_to_be_watched!$A$1:$I$43</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -202,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="73">
   <si>
     <t>Jana Struct TextureFeature Zuordnung</t>
   </si>
@@ -416,6 +417,38 @@
   <si>
     <t>strong_relevant p&lt;0,05</t>
   </si>
+  <si>
+    <r>
+      <t>significant_diff_in_val_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>significant_diff_in_val_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sim</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -497,7 +530,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,8 +600,20 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -882,6 +927,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -890,7 +965,7 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1039,6 +1114,14 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
@@ -2472,21 +2555,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C3EFAE-63B8-4ED6-8665-8A41871E76EB}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="13" customWidth="1"/>
-    <col min="3" max="10" width="12.7109375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" style="34" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="27"/>
+    <col min="2" max="2" width="12.6640625" style="13" customWidth="1"/>
+    <col min="3" max="10" width="12.6640625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="13" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" style="34" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -2530,7 +2613,7 @@
       </c>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -2571,7 +2654,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -2608,7 +2691,7 @@
       <c r="N3" s="29"/>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -2645,7 +2728,7 @@
       <c r="N4" s="29"/>
       <c r="O4" s="22"/>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>68</v>
       </c>
@@ -2682,7 +2765,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="23"/>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>61</v>
       </c>
@@ -2719,7 +2802,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="23"/>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>62</v>
       </c>
@@ -2756,7 +2839,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="23"/>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>67</v>
       </c>
@@ -2793,7 +2876,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="23"/>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>63</v>
       </c>
@@ -2830,7 +2913,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="23"/>
     </row>
-    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>64</v>
       </c>
@@ -2867,7 +2950,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>65</v>
       </c>
@@ -2904,7 +2987,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>66</v>
       </c>
@@ -2941,7 +3024,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="23"/>
     </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -2978,7 +3061,7 @@
       <c r="N13" s="31"/>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -3015,7 +3098,7 @@
       <c r="N14" s="31"/>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -3052,7 +3135,7 @@
       <c r="N15" s="31"/>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -3089,7 +3172,7 @@
       <c r="N16" s="31"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -3126,7 +3209,7 @@
       <c r="N17" s="31"/>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -3163,7 +3246,7 @@
       <c r="N18" s="31"/>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -3200,7 +3283,7 @@
       <c r="N19" s="31"/>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -3237,7 +3320,7 @@
       <c r="N20" s="31"/>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -3274,7 +3357,7 @@
       <c r="N21" s="31"/>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -3311,7 +3394,7 @@
       <c r="N22" s="31"/>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -3348,7 +3431,7 @@
       <c r="N23" s="32"/>
       <c r="O23" s="25"/>
     </row>
-    <row r="24" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -3385,7 +3468,7 @@
       <c r="N24" s="32"/>
       <c r="O24" s="25"/>
     </row>
-    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -3422,7 +3505,7 @@
       <c r="N25" s="32"/>
       <c r="O25" s="25"/>
     </row>
-    <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -3459,7 +3542,7 @@
       <c r="N26" s="31"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -3496,7 +3579,7 @@
       <c r="N27" s="31"/>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -3533,7 +3616,7 @@
       <c r="N28" s="31"/>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -3570,7 +3653,7 @@
       <c r="N29" s="32"/>
       <c r="O29" s="25"/>
     </row>
-    <row r="30" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -3607,7 +3690,7 @@
       <c r="N30" s="32"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -3644,7 +3727,7 @@
       <c r="N31" s="32"/>
       <c r="O31" s="25"/>
     </row>
-    <row r="32" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -3681,7 +3764,7 @@
       <c r="N32" s="32"/>
       <c r="O32" s="25"/>
     </row>
-    <row r="33" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -3718,7 +3801,7 @@
       <c r="N33" s="32"/>
       <c r="O33" s="25"/>
     </row>
-    <row r="34" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -3755,7 +3838,7 @@
       <c r="N34" s="32"/>
       <c r="O34" s="25"/>
     </row>
-    <row r="35" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -3792,7 +3875,7 @@
       <c r="N35" s="32"/>
       <c r="O35" s="25"/>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -3829,7 +3912,7 @@
       <c r="N36" s="32"/>
       <c r="O36" s="25"/>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -3866,7 +3949,7 @@
       <c r="N37" s="32"/>
       <c r="O37" s="25"/>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -3903,7 +3986,7 @@
       <c r="N38" s="32"/>
       <c r="O38" s="25"/>
     </row>
-    <row r="39" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -3940,7 +4023,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="26"/>
     </row>
-    <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -3977,7 +4060,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -4014,7 +4097,7 @@
       <c r="N41" s="33"/>
       <c r="O41" s="26"/>
     </row>
-    <row r="42" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -4051,7 +4134,7 @@
       <c r="N42" s="33"/>
       <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -4099,22 +4182,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEF64E8-C0CF-48B8-BA82-A098D67F4098}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="69" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="69" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="70" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" style="70" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" style="69" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="69" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="70" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" style="70" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="9" max="9" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
@@ -4126,8 +4213,16 @@
         <v>69</v>
       </c>
       <c r="E1" s="75"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="101" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="102"/>
+      <c r="H1" s="103" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="100"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
@@ -4145,8 +4240,22 @@
       <c r="E2" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="98" t="str">
+        <f>IF(G2&lt;&gt;0,"sig. Unterschied"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G2" s="98">
+        <v>0</v>
+      </c>
+      <c r="H2" s="99" t="str">
+        <f>IF(I2&lt;&gt;0,"sig. Unterschied"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I2" s="99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
@@ -4164,8 +4273,22 @@
       <c r="E3" s="80">
         <v>-0.84334340705856004</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="96" t="str">
+        <f t="shared" ref="F3:H43" si="2">IF(G3&lt;&gt;0,"sig. Unterschied"," ")</f>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G3" s="96">
+        <v>1</v>
+      </c>
+      <c r="H3" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I3" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="81" t="s">
         <v>3</v>
       </c>
@@ -4183,8 +4306,22 @@
       <c r="E4" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G4" s="96">
+        <v>1</v>
+      </c>
+      <c r="H4" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I4" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="79" t="s">
         <v>60</v>
       </c>
@@ -4202,8 +4339,22 @@
       <c r="E5" s="80">
         <v>0.98094415724929396</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G5" s="96">
+        <v>1</v>
+      </c>
+      <c r="H5" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I5" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
         <v>61</v>
       </c>
@@ -4221,8 +4372,22 @@
       <c r="E6" s="80">
         <v>0.90667141539436702</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G6" s="96">
+        <v>1</v>
+      </c>
+      <c r="H6" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I6" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>62</v>
       </c>
@@ -4240,8 +4405,22 @@
       <c r="E7" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G7" s="96">
+        <v>0</v>
+      </c>
+      <c r="H7" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I7" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="82" t="s">
         <v>67</v>
       </c>
@@ -4259,8 +4438,22 @@
       <c r="E8" s="80">
         <v>0.78863358261163596</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G8" s="96">
+        <v>1</v>
+      </c>
+      <c r="H8" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I8" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="83" t="s">
         <v>63</v>
       </c>
@@ -4278,8 +4471,22 @@
       <c r="E9" s="80">
         <v>0.94225755928788602</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G9" s="96">
+        <v>1</v>
+      </c>
+      <c r="H9" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I9" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="82" t="s">
         <v>64</v>
       </c>
@@ -4297,8 +4504,22 @@
       <c r="E10" s="80">
         <v>0.983464848574366</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G10" s="96">
+        <v>0</v>
+      </c>
+      <c r="H10" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I10" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="83" t="s">
         <v>65</v>
       </c>
@@ -4316,8 +4537,22 @@
       <c r="E11" s="80">
         <v>0.96852446011525595</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G11" s="96">
+        <v>1</v>
+      </c>
+      <c r="H11" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I11" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="82" t="s">
         <v>66</v>
       </c>
@@ -4335,8 +4570,22 @@
       <c r="E12" s="80">
         <v>0.880414083092942</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G12" s="96">
+        <v>1</v>
+      </c>
+      <c r="H12" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I12" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="84" t="s">
         <v>12</v>
       </c>
@@ -4354,8 +4603,22 @@
       <c r="E13" s="80">
         <v>0.59865021210115799</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G13" s="96">
+        <v>0</v>
+      </c>
+      <c r="H13" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I13" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="84" t="s">
         <v>13</v>
       </c>
@@ -4373,8 +4636,22 @@
       <c r="E14" s="80">
         <v>0.65352193986602303</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G14" s="96">
+        <v>0</v>
+      </c>
+      <c r="H14" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I14" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="84" t="s">
         <v>14</v>
       </c>
@@ -4392,8 +4669,22 @@
       <c r="E15" s="80">
         <v>0.97674279578822198</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G15" s="96">
+        <v>1</v>
+      </c>
+      <c r="H15" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I15" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="84" t="s">
         <v>15</v>
       </c>
@@ -4411,8 +4702,22 @@
       <c r="E16" s="80">
         <v>0.58878704386803604</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G16" s="96">
+        <v>0</v>
+      </c>
+      <c r="H16" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I16" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="84" t="s">
         <v>16</v>
       </c>
@@ -4430,8 +4735,22 @@
       <c r="E17" s="80">
         <v>0.62505964320140095</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G17" s="96">
+        <v>0</v>
+      </c>
+      <c r="H17" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I17" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="85" t="s">
         <v>17</v>
       </c>
@@ -4449,8 +4768,22 @@
       <c r="E18" s="80">
         <v>-0.96788888686397101</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G18" s="96">
+        <v>0</v>
+      </c>
+      <c r="H18" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I18" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="84" t="s">
         <v>18</v>
       </c>
@@ -4468,8 +4801,22 @@
       <c r="E19" s="80">
         <v>0.97351887955009098</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G19" s="96">
+        <v>1</v>
+      </c>
+      <c r="H19" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I19" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="84" t="s">
         <v>19</v>
       </c>
@@ -4487,8 +4834,22 @@
       <c r="E20" s="80">
         <v>0.96059237873661696</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G20" s="96">
+        <v>1</v>
+      </c>
+      <c r="H20" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I20" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="84" t="s">
         <v>20</v>
       </c>
@@ -4506,8 +4867,22 @@
       <c r="E21" s="80">
         <v>0.92409378832753297</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G21" s="96">
+        <v>1</v>
+      </c>
+      <c r="H21" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I21" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="84" t="s">
         <v>21</v>
       </c>
@@ -4525,8 +4900,22 @@
       <c r="E22" s="80">
         <v>0.99973594679469802</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G22" s="96">
+        <v>1</v>
+      </c>
+      <c r="H22" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I22" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="86" t="s">
         <v>22</v>
       </c>
@@ -4544,8 +4933,22 @@
       <c r="E23" s="80">
         <v>0.71849382730993205</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G23" s="96">
+        <v>1</v>
+      </c>
+      <c r="H23" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I23" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="87" t="s">
         <v>23</v>
       </c>
@@ -4563,8 +4966,22 @@
       <c r="E24" s="80">
         <v>0.64996905256680304</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G24" s="96">
+        <v>1</v>
+      </c>
+      <c r="H24" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I24" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="87" t="s">
         <v>24</v>
       </c>
@@ -4582,8 +4999,22 @@
       <c r="E25" s="80">
         <v>0.93343263907822105</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G25" s="96">
+        <v>1</v>
+      </c>
+      <c r="H25" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I25" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="84" t="s">
         <v>25</v>
       </c>
@@ -4601,8 +5032,22 @@
       <c r="E26" s="80">
         <v>-0.98373744652900696</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G26" s="96">
+        <v>1</v>
+      </c>
+      <c r="H26" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I26" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="84" t="s">
         <v>26</v>
       </c>
@@ -4620,8 +5065,22 @@
       <c r="E27" s="80">
         <v>0.97598760147302799</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G27" s="96">
+        <v>1</v>
+      </c>
+      <c r="H27" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I27" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="84" t="s">
         <v>27</v>
       </c>
@@ -4639,8 +5098,22 @@
       <c r="E28" s="80">
         <v>0.921403954645723</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G28" s="96">
+        <v>0</v>
+      </c>
+      <c r="H28" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I28" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="88" t="s">
         <v>28</v>
       </c>
@@ -4658,8 +5131,22 @@
       <c r="E29" s="80">
         <v>0.70938857081172502</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G29" s="96">
+        <v>1</v>
+      </c>
+      <c r="H29" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I29" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="87" t="s">
         <v>29</v>
       </c>
@@ -4677,8 +5164,22 @@
       <c r="E30" s="80">
         <v>0.53021105748659303</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G30" s="96">
+        <v>1</v>
+      </c>
+      <c r="H30" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I30" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="79" t="s">
         <v>30</v>
       </c>
@@ -4696,8 +5197,22 @@
       <c r="E31" s="80">
         <v>0.50402048293739898</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G31" s="96">
+        <v>1</v>
+      </c>
+      <c r="H31" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I31" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="89" t="s">
         <v>31</v>
       </c>
@@ -4715,8 +5230,22 @@
       <c r="E32" s="80">
         <v>0.98640124814101904</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G32" s="96">
+        <v>1</v>
+      </c>
+      <c r="H32" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I32" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="79" t="s">
         <v>32</v>
       </c>
@@ -4734,8 +5263,22 @@
       <c r="E33" s="80">
         <v>0.87951332144286598</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G33" s="96">
+        <v>1</v>
+      </c>
+      <c r="H33" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I33" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="90" t="s">
         <v>33</v>
       </c>
@@ -4753,8 +5296,22 @@
       <c r="E34" s="80">
         <v>0.98441429728291097</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G34" s="96">
+        <v>1</v>
+      </c>
+      <c r="H34" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I34" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="90" t="s">
         <v>34</v>
       </c>
@@ -4772,8 +5329,22 @@
       <c r="E35" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G35" s="96">
+        <v>1</v>
+      </c>
+      <c r="H35" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I35" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="90" t="s">
         <v>35</v>
       </c>
@@ -4791,8 +5362,22 @@
       <c r="E36" s="80">
         <v>-0.84437614994385801</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G36" s="96">
+        <v>1</v>
+      </c>
+      <c r="H36" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I36" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="90" t="s">
         <v>36</v>
       </c>
@@ -4810,8 +5395,22 @@
       <c r="E37" s="80">
         <v>0.88985847317508604</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G37" s="96">
+        <v>1</v>
+      </c>
+      <c r="H37" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I37" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="90" t="s">
         <v>37</v>
       </c>
@@ -4829,8 +5428,22 @@
       <c r="E38" s="80">
         <v>-0.55957873713127604</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G38" s="96">
+        <v>1</v>
+      </c>
+      <c r="H38" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I38" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="91" t="s">
         <v>38</v>
       </c>
@@ -4848,8 +5461,22 @@
       <c r="E39" s="80">
         <v>0.59984490126308398</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G39" s="96">
+        <v>1</v>
+      </c>
+      <c r="H39" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I39" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="91" t="s">
         <v>39</v>
       </c>
@@ -4867,8 +5494,22 @@
       <c r="E40" s="80">
         <v>0.94939894857966201</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G40" s="96">
+        <v>1</v>
+      </c>
+      <c r="H40" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I40" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="91" t="s">
         <v>40</v>
       </c>
@@ -4886,8 +5527,22 @@
       <c r="E41" s="80">
         <v>0.887779232640306</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G41" s="96">
+        <v>1</v>
+      </c>
+      <c r="H41" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I41" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="91" t="s">
         <v>41</v>
       </c>
@@ -4905,8 +5560,22 @@
       <c r="E42" s="80">
         <v>0.97753699258675497</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G42" s="96">
+        <v>1</v>
+      </c>
+      <c r="H42" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I42" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="92" t="s">
         <v>42</v>
       </c>
@@ -4924,8 +5593,22 @@
       <c r="E43" s="95">
         <v>0.79491795524470799</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="96" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="G43" s="96">
+        <v>1</v>
+      </c>
+      <c r="H43" s="97" t="str">
+        <f t="shared" si="2"/>
+        <v>sig. Unterschied</v>
+      </c>
+      <c r="I43" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B44" s="71"/>
       <c r="C44" s="71"/>
       <c r="D44" s="72"/>
@@ -4942,19 +5625,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8176F4A9-4881-448D-A0E0-F9B6D997CC24}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="60" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="62" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="60" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -4965,7 +5648,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -4980,7 +5663,7 @@
         <v>0.22100390029524827</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
@@ -4995,7 +5678,7 @@
         <v>-20.738395527237444</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -5010,7 +5693,7 @@
         <v>-2.8374759913231831</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
         <v>57</v>
       </c>
@@ -5025,7 +5708,7 @@
         <v>1.5289763834216858</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="53" t="s">
         <v>5</v>
       </c>
@@ -5040,7 +5723,7 @@
         <v>2.9628655086972087</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="53" t="s">
         <v>6</v>
       </c>
@@ -5055,7 +5738,7 @@
         <v>0.96632496296385195</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="55" t="s">
         <v>7</v>
       </c>
@@ -5070,7 +5753,7 @@
         <v>0.98047604427471413</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -5085,7 +5768,7 @@
         <v>0.81663098920756272</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="55" t="s">
         <v>9</v>
       </c>
@@ -5100,7 +5783,7 @@
         <v>0.8915843690456291</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -5115,7 +5798,7 @@
         <v>1.8538821007245201</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="55" t="s">
         <v>11</v>
       </c>
@@ -5130,7 +5813,7 @@
         <v>2.5799069109485777</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -5145,7 +5828,7 @@
         <v>8.1141674582550873</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -5160,7 +5843,7 @@
         <v>0.6730437252298882</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -5175,7 +5858,7 @@
         <v>0.53079394521493595</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -5190,7 +5873,7 @@
         <v>4.731792326014487</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -5205,7 +5888,7 @@
         <v>1.7005796902810768</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -5220,7 +5903,7 @@
         <v>0.65559777286450649</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -5235,7 +5918,7 @@
         <v>2.6986414747414047</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -5250,7 +5933,7 @@
         <v>0.25976781062598786</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -5265,7 +5948,7 @@
         <v>13.372416259839857</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -5280,7 +5963,7 @@
         <v>0.61038626160105325</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="54" t="s">
         <v>22</v>
       </c>
@@ -5295,7 +5978,7 @@
         <v>10857807428.36091</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -5310,7 +5993,7 @@
         <v>1.1401258236302761E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -5325,7 +6008,7 @@
         <v>0.75224966808175997</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -5340,7 +6023,7 @@
         <v>2.7117620565402185</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -5355,7 +6038,7 @@
         <v>28.081324955208988</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -5370,7 +6053,7 @@
         <v>1.251657275145535</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="56" t="s">
         <v>28</v>
       </c>
@@ -5385,7 +6068,7 @@
         <v>0.35466898326476398</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -5400,7 +6083,7 @@
         <v>124.71569979779608</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="53" t="s">
         <v>30</v>
       </c>
@@ -5415,7 +6098,7 @@
         <v>0.4856050382366176</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="57" t="s">
         <v>31</v>
       </c>
@@ -5430,7 +6113,7 @@
         <v>4.1538461538461595</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
         <v>32</v>
       </c>
@@ -5445,7 +6128,7 @@
         <v>3746612192.0750699</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -5460,7 +6143,7 @@
         <v>54431080203.797195</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -5475,7 +6158,7 @@
         <v>1.9515437015490144E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -5490,7 +6173,7 @@
         <v>4.5640310354127748E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -5505,7 +6188,7 @@
         <v>0.5669448606432177</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -5520,7 +6203,7 @@
         <v>5.865728178013417E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -5535,7 +6218,7 @@
         <v>1.7834100925449967</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -5550,7 +6233,7 @@
         <v>0.76630452864961585</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -5565,7 +6248,7 @@
         <v>0.14445492813477548</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -5580,7 +6263,7 @@
         <v>8.4496932746363491</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -5609,17 +6292,17 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="27"/>
+    <col min="2" max="2" width="12.6640625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -5641,7 +6324,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -5658,7 +6341,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -5671,7 +6354,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -5684,7 +6367,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -5697,7 +6380,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -5710,7 +6393,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -5723,7 +6406,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -5736,7 +6419,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -5749,7 +6432,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -5762,7 +6445,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -5775,7 +6458,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -5788,7 +6471,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -5801,7 +6484,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -5814,7 +6497,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -5827,7 +6510,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -5840,7 +6523,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -5853,7 +6536,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -5866,7 +6549,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -5879,7 +6562,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -5892,7 +6575,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -5905,7 +6588,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -5918,7 +6601,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -5931,7 +6614,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -5944,7 +6627,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -5957,7 +6640,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -5970,7 +6653,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -5983,7 +6666,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -5996,7 +6679,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -6009,7 +6692,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -6022,7 +6705,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -6035,7 +6718,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -6048,7 +6731,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -6061,7 +6744,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -6074,7 +6757,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -6087,7 +6770,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -6100,7 +6783,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -6113,7 +6796,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -6126,7 +6809,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -6139,7 +6822,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -6152,7 +6835,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -6165,7 +6848,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -6178,7 +6861,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -6208,16 +6891,16 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="27"/>
+    <col min="2" max="3" width="12.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -6239,7 +6922,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -6256,7 +6939,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -6269,7 +6952,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -6282,7 +6965,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -6295,7 +6978,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -6308,7 +6991,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -6321,7 +7004,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -6334,7 +7017,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -6347,7 +7030,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -6360,7 +7043,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -6373,7 +7056,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -6386,7 +7069,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -6399,7 +7082,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -6412,7 +7095,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -6425,7 +7108,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -6438,7 +7121,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -6451,7 +7134,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -6464,7 +7147,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -6477,7 +7160,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -6490,7 +7173,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -6503,7 +7186,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -6516,7 +7199,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -6529,7 +7212,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -6542,7 +7225,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -6555,7 +7238,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -6568,7 +7251,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -6581,7 +7264,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -6594,7 +7277,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -6607,7 +7290,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -6620,7 +7303,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -6633,7 +7316,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -6646,7 +7329,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -6659,7 +7342,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -6672,7 +7355,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -6685,7 +7368,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -6698,7 +7381,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -6711,7 +7394,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -6724,7 +7407,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -6737,7 +7420,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -6750,7 +7433,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -6763,7 +7446,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -6776,7 +7459,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -6806,16 +7489,16 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="27"/>
+    <col min="2" max="3" width="12.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -6837,7 +7520,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -6854,7 +7537,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -6867,7 +7550,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -6880,7 +7563,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -6893,7 +7576,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -6906,7 +7589,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -6919,7 +7602,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -6932,7 +7615,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -6945,7 +7628,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -6958,7 +7641,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -6971,7 +7654,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -6984,7 +7667,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -6997,7 +7680,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -7010,7 +7693,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -7023,7 +7706,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -7036,7 +7719,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -7049,7 +7732,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -7062,7 +7745,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -7075,7 +7758,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -7088,7 +7771,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -7101,7 +7784,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -7114,7 +7797,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -7127,7 +7810,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -7140,7 +7823,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -7153,7 +7836,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -7166,7 +7849,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -7179,7 +7862,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -7192,7 +7875,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -7205,7 +7888,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -7218,7 +7901,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -7231,7 +7914,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -7244,7 +7927,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -7257,7 +7940,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -7270,7 +7953,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -7283,7 +7966,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -7296,7 +7979,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -7309,7 +7992,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -7322,7 +8005,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -7335,7 +8018,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -7348,7 +8031,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -7361,7 +8044,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -7374,7 +8057,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -7404,16 +8087,16 @@
       <selection activeCell="B2" sqref="B2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="27"/>
+    <col min="2" max="3" width="12.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -7435,7 +8118,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -7452,7 +8135,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -7465,7 +8148,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -7478,7 +8161,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -7491,7 +8174,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -7504,7 +8187,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -7517,7 +8200,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -7530,7 +8213,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -7543,7 +8226,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -7556,7 +8239,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -7569,7 +8252,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -7582,7 +8265,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -7595,7 +8278,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -7608,7 +8291,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -7621,7 +8304,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -7634,7 +8317,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -7647,7 +8330,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -7660,7 +8343,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -7673,7 +8356,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -7686,7 +8369,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -7699,7 +8382,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -7712,7 +8395,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -7725,7 +8408,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -7738,7 +8421,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -7751,7 +8434,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -7764,7 +8447,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -7777,7 +8460,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -7790,7 +8473,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -7803,7 +8486,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -7816,7 +8499,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -7829,7 +8512,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -7842,7 +8525,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -7855,7 +8538,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -7868,7 +8551,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -7881,7 +8564,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -7894,7 +8577,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -7907,7 +8590,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -7920,7 +8603,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -7933,7 +8616,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -7946,7 +8629,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -7959,7 +8642,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -7972,7 +8655,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -8002,17 +8685,17 @@
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="19" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="52" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="27"/>
+    <col min="2" max="2" width="12.6640625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="52" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -8034,7 +8717,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -8051,7 +8734,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -8064,7 +8747,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -8077,7 +8760,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>4</v>
       </c>
@@ -8090,7 +8773,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
@@ -8103,7 +8786,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
@@ -8116,7 +8799,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
@@ -8129,7 +8812,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -8142,7 +8825,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
@@ -8155,7 +8838,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>10</v>
       </c>
@@ -8168,7 +8851,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
@@ -8181,7 +8864,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
@@ -8194,7 +8877,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
@@ -8207,7 +8890,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
@@ -8220,7 +8903,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -8233,7 +8916,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -8246,7 +8929,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>17</v>
       </c>
@@ -8259,7 +8942,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
@@ -8272,7 +8955,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
@@ -8285,7 +8968,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>20</v>
       </c>
@@ -8298,7 +8981,7 @@
       <c r="F21" s="31"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>21</v>
       </c>
@@ -8311,7 +8994,7 @@
       <c r="F22" s="31"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -8324,7 +9007,7 @@
       <c r="F23" s="32"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>23</v>
       </c>
@@ -8337,7 +9020,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>24</v>
       </c>
@@ -8350,7 +9033,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>25</v>
       </c>
@@ -8363,7 +9046,7 @@
       <c r="F26" s="31"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>26</v>
       </c>
@@ -8376,7 +9059,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>27</v>
       </c>
@@ -8389,7 +9072,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -8402,7 +9085,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
@@ -8415,7 +9098,7 @@
       <c r="F30" s="32"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
@@ -8428,7 +9111,7 @@
       <c r="F31" s="32"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
@@ -8441,7 +9124,7 @@
       <c r="F32" s="32"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -8454,7 +9137,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
         <v>33</v>
       </c>
@@ -8467,7 +9150,7 @@
       <c r="F34" s="32"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
@@ -8480,7 +9163,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40" t="s">
         <v>35</v>
       </c>
@@ -8493,7 +9176,7 @@
       <c r="F36" s="32"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40" t="s">
         <v>36</v>
       </c>
@@ -8506,7 +9189,7 @@
       <c r="F37" s="32"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
         <v>37</v>
       </c>
@@ -8519,7 +9202,7 @@
       <c r="F38" s="32"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>38</v>
       </c>
@@ -8532,7 +9215,7 @@
       <c r="F39" s="33"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>39</v>
       </c>
@@ -8545,7 +9228,7 @@
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -8558,7 +9241,7 @@
       <c r="F41" s="33"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -8571,7 +9254,7 @@
       <c r="F42" s="33"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
nii and multiple dirs
</commit_message>
<xml_diff>
--- a/Matthias/01-NEMA_Phantom/Measured_vs_Simulated_allDosis_Mask_TK.xlsx
+++ b/Matthias/01-NEMA_Phantom/Measured_vs_Simulated_allDosis_Mask_TK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\TAToolbox\Matthias\01-NEMA_Phantom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391EA5BA-6836-45FC-831D-D68F53510FA3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8C7725-46B3-4FAE-9587-A1FBEC27C22C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6996" tabRatio="703" activeTab="2" xr2:uid="{CEAB1AE0-CCC6-4F1C-87B6-462A97D959FC}"/>
   </bookViews>
@@ -5626,7 +5626,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>